<commit_message>
moved some auto generated files to gitignore, added design docs
</commit_message>
<xml_diff>
--- a/Design Docs/ASB Power Calcs.xlsx
+++ b/Design Docs/ASB Power Calcs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE40EC1-9117-4047-844A-57E3B40F3411}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5B20B9-77E2-421D-B657-F1E05B5559BF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>12V Supply</t>
   </si>
@@ -44,6 +44,24 @@
   </si>
   <si>
     <t>Temperature Sensor x 12</t>
+  </si>
+  <si>
+    <t>Current Sensor x 6</t>
+  </si>
+  <si>
+    <t>5V Supply</t>
+  </si>
+  <si>
+    <t>CAN Transceiver</t>
+  </si>
+  <si>
+    <t>External ADC</t>
+  </si>
+  <si>
+    <t>Gigavac contactor</t>
+  </si>
+  <si>
+    <t>Omron Relay x 2</t>
   </si>
 </sst>
 </file>
@@ -370,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -381,11 +399,13 @@
     <col min="1" max="1" width="21.53125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.73046875" customWidth="1"/>
-    <col min="4" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -399,16 +419,32 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>250</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <f>25*6</f>
+        <v>150</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -416,13 +452,36 @@
         <f>4*3</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <f>100*2</f>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>